<commit_message>
Processed Results - nexus 5x until gps
</commit_message>
<xml_diff>
--- a/Processed Results/Nexus 5X/Cpu/Cpu - Processed.xlsx
+++ b/Processed Results/Nexus 5X/Cpu/Cpu - Processed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Nexus 5X\Cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB13438-FF3F-4E0D-8779-9CF5507A8148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9559D4D-DFD3-4E24-87EC-91682A7E72B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
@@ -16,16 +16,18 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$2:$A$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$98:$A$187</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$98:$B$187</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$A$34:$A$63</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$B$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$34:$B$63</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$A$66:$A$95</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$B$65</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$98:$A$187</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$98:$B$187</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Blad1!$A$98:$A$187</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Blad1!$B$98:$B$187</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$34:$A$63</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$33</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$B$34:$B$63</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$A$66:$A$95</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$65</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$A$2:$A$31</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$2:$B$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -283,94 +285,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>108.467891999999</c:v>
+                  <c:v>122.01944399999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104.53219199999999</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.800484</c:v>
+                  <c:v>123.585804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102.95791199999999</c:v>
+                  <c:v>124.838892</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.95791199999999</c:v>
+                  <c:v>124.055712</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>101.226204</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102.48562800000001</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>101.698488</c:v>
+                  <c:v>123.115895999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>101.54106</c:v>
+                  <c:v>124.21234800000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>101.85591599999999</c:v>
+                  <c:v>124.055712</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101.85591599999999</c:v>
+                  <c:v>122.95926</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>102.170772</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>101.54106</c:v>
+                  <c:v>124.055712</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>101.54106</c:v>
+                  <c:v>123.89907599999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>101.698488</c:v>
+                  <c:v>124.682256</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>116.969004</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>102.95791199999999</c:v>
+                  <c:v>123.115895999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>101.85591599999999</c:v>
+                  <c:v>123.429167999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>101.54106</c:v>
+                  <c:v>124.368984</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>102.3282</c:v>
+                  <c:v>124.52562</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>102.170772</c:v>
+                  <c:v>123.115895999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>102.48562800000001</c:v>
+                  <c:v>123.429167999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>102.643056</c:v>
+                  <c:v>124.055712</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>103.587623999999</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>101.85591599999999</c:v>
+                  <c:v>122.489352</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>101.54106</c:v>
+                  <c:v>123.89907599999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>101.698488</c:v>
+                  <c:v>122.489352</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>102.013344</c:v>
+                  <c:v>123.585804</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>101.38363200000001</c:v>
+                  <c:v>119.043359999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>102.3282</c:v>
+                  <c:v>123.429167999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,10 +448,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>102.88969319999993</c:v>
+                  <c:v>124.07137559999973</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.88969319999993</c:v>
+                  <c:v>124.07137559999973</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,94 +912,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>105.584256</c:v>
+                  <c:v>127.814976</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105.74208</c:v>
+                  <c:v>134.70695999999899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>105.74208</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.110784</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.26860799999901</c:v>
+                  <c:v>127.97161199999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.110784</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.584256</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>104.795136</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104.795136</c:v>
+                  <c:v>128.44152</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>104.479488</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105.26860799999901</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>106.84684799999999</c:v>
+                  <c:v>124.838892</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105.74208</c:v>
+                  <c:v>136.89986399999901</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>106.057728</c:v>
+                  <c:v>128.59815599999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.110784</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>105.426431999999</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104.95296</c:v>
+                  <c:v>128.28488399999901</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>105.426431999999</c:v>
+                  <c:v>127.814976</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>104.795136</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>104.95296</c:v>
+                  <c:v>128.75479200000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>104.95296</c:v>
+                  <c:v>132.98396399999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>105.584256</c:v>
+                  <c:v>128.44152</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>104.95296</c:v>
+                  <c:v>129.537972</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>105.426431999999</c:v>
+                  <c:v>131.104332</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>104.795136</c:v>
+                  <c:v>130.32115200000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>105.110784</c:v>
+                  <c:v>134.23705200000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>105.110784</c:v>
+                  <c:v>129.06806399999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>105.110784</c:v>
+                  <c:v>133.297236</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>104.16383999999999</c:v>
+                  <c:v>124.52562</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>105.89990400000001</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1049,10 +1051,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>105.26334719999984</c:v>
+                  <c:v>129.5327507999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105.26334719999984</c:v>
+                  <c:v>129.5327507999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,94 +1606,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>113.401224</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114.83265599999901</c:v>
+                  <c:v>145.82811599999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114.83265599999901</c:v>
+                  <c:v>144.88829999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>118.967904</c:v>
+                  <c:v>145.35820799999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>112.605983999999</c:v>
+                  <c:v>147.394476</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>114.83265599999901</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.87836799999999</c:v>
+                  <c:v>144.105119999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113.87836799999999</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>114.03741599999999</c:v>
+                  <c:v>143.635212</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>113.24217599999901</c:v>
+                  <c:v>146.92456799999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>114.991704</c:v>
+                  <c:v>145.67148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>114.51456</c:v>
+                  <c:v>142.69539599999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>114.83265599999901</c:v>
+                  <c:v>145.201572</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>114.03741599999999</c:v>
+                  <c:v>144.575028</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>114.51456</c:v>
+                  <c:v>145.35820799999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>114.03741599999999</c:v>
+                  <c:v>144.73166399999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>113.401224</c:v>
+                  <c:v>146.14138800000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>113.71932</c:v>
+                  <c:v>150.213923999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>113.87836799999999</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113.71932</c:v>
+                  <c:v>143.635212</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>114.03741599999999</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>114.196463999999</c:v>
+                  <c:v>143.79184799999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>114.67360799999901</c:v>
+                  <c:v>143.635212</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>115.150752</c:v>
+                  <c:v>145.201572</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>113.71932</c:v>
+                  <c:v>145.04493600000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>113.87836799999999</c:v>
+                  <c:v>145.04493600000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>116.90028</c:v>
+                  <c:v>144.105119999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>112.605983999999</c:v>
+                  <c:v>143.478576</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>114.51456</c:v>
+                  <c:v>144.26175599999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>113.71932</c:v>
+                  <c:v>144.41839200000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1743,10 +1745,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>114.31840079999974</c:v>
+                  <c:v>144.88829999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114.31840079999974</c:v>
+                  <c:v>144.88829999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1890,7 +1892,6 @@
         <c:axId val="281410968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="119"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2092,10 +2093,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2171,7 +2172,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="118" min="99"/>
+        <cx:valScaling min="118"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2214,10 +2215,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2292,7 +2293,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling min="100"/>
+        <cx:valScaling min="118"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2335,10 +2336,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2376,7 +2377,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3F5A16A3-6E4C-4475-A634-1322A70DC713}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Medium_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2420,7 +2421,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling min="103.5"/>
+        <cx:valScaling min="122"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2463,10 +2464,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2504,7 +2505,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{138ACD3C-CAEA-4AEF-B3DF-B982F1EA92CC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>High_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2548,7 +2549,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling min="110"/>
+        <cx:valScaling max="151" min="142"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -7198,8 +7199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FE0459-F6C0-45BE-AD60-56F63431C3F0}">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7222,7 +7223,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>108.467891999999</v>
+        <v>122.01944399999999</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
@@ -7236,14 +7237,14 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>104.53219199999999</v>
+        <v>129.537972</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>102.88969319999993</v>
+        <v>124.07137559999973</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -7251,14 +7252,14 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>102.800484</v>
+        <v>123.585804</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>102.88969319999993</v>
+        <v>124.07137559999973</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -7266,7 +7267,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>102.95791199999999</v>
+        <v>124.838892</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -7274,7 +7275,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>102.95791199999999</v>
+        <v>124.055712</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -7288,15 +7289,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>101.226204</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="D7" s="1">
         <f>MIN(B2:B31)</f>
-        <v>101.226204</v>
+        <v>119.043359999999</v>
       </c>
       <c r="E7" s="1">
         <f>MAX(B2:B31)</f>
-        <v>116.969004</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -7304,7 +7305,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>102.48562800000001</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -7312,7 +7313,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>101.698488</v>
+        <v>123.115895999999</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -7326,15 +7327,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>101.54106</v>
+        <v>124.21234800000001</v>
       </c>
       <c r="D10">
         <f>QUARTILE(B2:B31, 1)</f>
-        <v>101.698488</v>
+        <v>123.115895999999</v>
       </c>
       <c r="E10">
         <f>QUARTILE(B2:B31, 2)</f>
-        <v>102.09205800000001</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -7342,7 +7343,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>101.85591599999999</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -7350,7 +7351,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>101.85591599999999</v>
+        <v>122.95926</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -7364,15 +7365,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>102.170772</v>
+        <v>119.82653999999999</v>
       </c>
       <c r="D13">
         <f>QUARTILE(B2:B31, 3)</f>
-        <v>102.761127</v>
+        <v>124.48646100000001</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> D13 - D10</f>
-        <v>1.0626390000000043</v>
+        <v>1.3705650000010081</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -7380,7 +7381,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>101.54106</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -7388,7 +7389,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>101.54106</v>
+        <v>123.89907599999999</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -7402,15 +7403,15 @@
         <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>101.698488</v>
+        <v>124.682256</v>
       </c>
       <c r="D16">
         <f>STDEV(B2:B31)</f>
-        <v>2.9828873338770054</v>
+        <v>2.2045820248040093</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (D16 / E4) * 100</f>
-        <v>2.899111894598406</v>
+        <v>1.7768659484452547</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -7418,7 +7419,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>116.969004</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -7426,7 +7427,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1">
-        <v>102.95791199999999</v>
+        <v>123.115895999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -7434,7 +7435,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="1">
-        <v>101.85591599999999</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7442,7 +7443,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>101.54106</v>
+        <v>124.368984</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -7450,7 +7451,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1">
-        <v>102.3282</v>
+        <v>124.52562</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -7458,7 +7459,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1">
-        <v>102.170772</v>
+        <v>123.115895999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -7466,7 +7467,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="1">
-        <v>102.48562800000001</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -7474,7 +7475,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <v>102.643056</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -7482,7 +7483,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>103.587623999999</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -7490,7 +7491,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="1">
-        <v>101.85591599999999</v>
+        <v>122.489352</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -7498,7 +7499,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1">
-        <v>101.54106</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -7506,7 +7507,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="1">
-        <v>101.698488</v>
+        <v>122.489352</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -7514,7 +7515,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="1">
-        <v>102.013344</v>
+        <v>123.585804</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -7522,7 +7523,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1">
-        <v>101.38363200000001</v>
+        <v>119.043359999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -7530,7 +7531,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="1">
-        <v>102.3282</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -7549,7 +7550,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="1">
-        <v>105.584256</v>
+        <v>127.814976</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -7563,14 +7564,14 @@
         <v>12</v>
       </c>
       <c r="B35" s="1">
-        <v>105.74208</v>
+        <v>134.70695999999899</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>105.26334719999984</v>
+        <v>129.5327507999998</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -7578,14 +7579,14 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <v>105.74208</v>
+        <v>128.59815599999999</v>
       </c>
       <c r="D36">
         <v>30</v>
       </c>
       <c r="E36" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>105.26334719999984</v>
+        <v>129.5327507999998</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -7593,7 +7594,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="1">
-        <v>105.110784</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -7601,7 +7602,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="1">
-        <v>105.26860799999901</v>
+        <v>127.97161199999999</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>3</v>
@@ -7615,15 +7616,15 @@
         <v>12</v>
       </c>
       <c r="B39" s="1">
-        <v>105.110784</v>
+        <v>129.537972</v>
       </c>
       <c r="D39" s="1">
         <f>MIN(B34:B63)</f>
-        <v>104.16383999999999</v>
+        <v>124.52562</v>
       </c>
       <c r="E39" s="1">
         <f>MAX(B34:B63)</f>
-        <v>106.84684799999999</v>
+        <v>136.89986399999901</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -7631,7 +7632,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="1">
-        <v>105.584256</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -7639,7 +7640,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="1">
-        <v>104.795136</v>
+        <v>128.59815599999999</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
@@ -7653,15 +7654,15 @@
         <v>12</v>
       </c>
       <c r="B42" s="1">
-        <v>104.795136</v>
+        <v>128.44152</v>
       </c>
       <c r="D42">
         <f>QUARTILE(B34:B63, 1)</f>
-        <v>104.95296</v>
+        <v>128.32404299999925</v>
       </c>
       <c r="E42">
         <f>QUARTILE(B34:B63, 2)</f>
-        <v>105.110784</v>
+        <v>128.911428</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -7669,7 +7670,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="1">
-        <v>104.479488</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -7677,7 +7678,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="1">
-        <v>105.26860799999901</v>
+        <v>129.537972</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -7691,15 +7692,15 @@
         <v>12</v>
       </c>
       <c r="B45" s="1">
-        <v>106.84684799999999</v>
+        <v>124.838892</v>
       </c>
       <c r="D45">
         <f>QUARTILE(B34:B63, 3)</f>
-        <v>105.584256</v>
+        <v>129.537972</v>
       </c>
       <c r="E45">
         <f xml:space="preserve"> D45 - D42</f>
-        <v>0.63129599999999186</v>
+        <v>1.2139290000007463</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -7707,7 +7708,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="1">
-        <v>105.74208</v>
+        <v>136.89986399999901</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -7715,7 +7716,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="1">
-        <v>106.057728</v>
+        <v>128.59815599999999</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>16</v>
@@ -7729,15 +7730,15 @@
         <v>12</v>
       </c>
       <c r="B48" s="1">
-        <v>105.110784</v>
+        <v>129.22469999999899</v>
       </c>
       <c r="D48">
         <f>STDEV(B34:B63)</f>
-        <v>0.52012334203432764</v>
+        <v>2.6279469664054198</v>
       </c>
       <c r="E48">
         <f xml:space="preserve"> (D48 / E36) * 100</f>
-        <v>0.49411628631388266</v>
+        <v>2.0287895919565568</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -7745,7 +7746,7 @@
         <v>12</v>
       </c>
       <c r="B49" s="1">
-        <v>105.426431999999</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -7753,7 +7754,7 @@
         <v>12</v>
       </c>
       <c r="B50" s="1">
-        <v>104.95296</v>
+        <v>128.28488399999901</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -7761,7 +7762,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="1">
-        <v>105.426431999999</v>
+        <v>127.814976</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -7769,7 +7770,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="1">
-        <v>104.795136</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -7777,7 +7778,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="1">
-        <v>104.95296</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -7785,7 +7786,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="1">
-        <v>104.95296</v>
+        <v>132.98396399999999</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -7793,7 +7794,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="1">
-        <v>105.584256</v>
+        <v>128.44152</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -7801,7 +7802,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="1">
-        <v>104.95296</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -7809,7 +7810,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="1">
-        <v>105.426431999999</v>
+        <v>131.104332</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -7817,7 +7818,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1">
-        <v>104.795136</v>
+        <v>130.32115200000001</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -7825,7 +7826,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="1">
-        <v>105.110784</v>
+        <v>134.23705200000001</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -7833,7 +7834,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="1">
-        <v>105.110784</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -7841,7 +7842,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="1">
-        <v>105.110784</v>
+        <v>133.297236</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -7849,7 +7850,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="1">
-        <v>104.16383999999999</v>
+        <v>124.52562</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -7857,7 +7858,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="1">
-        <v>105.89990400000001</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -7876,7 +7877,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="1">
-        <v>113.401224</v>
+        <v>144.26175599999999</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -7890,14 +7891,14 @@
         <v>14</v>
       </c>
       <c r="B67" s="1">
-        <v>114.83265599999901</v>
+        <v>145.82811599999999</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>114.31840079999974</v>
+        <v>144.88829999999987</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -7905,14 +7906,14 @@
         <v>14</v>
       </c>
       <c r="B68" s="1">
-        <v>114.83265599999901</v>
+        <v>144.88829999999999</v>
       </c>
       <c r="D68">
         <v>30</v>
       </c>
       <c r="E68" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>114.31840079999974</v>
+        <v>144.88829999999987</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -7920,7 +7921,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="1">
-        <v>118.967904</v>
+        <v>145.35820799999999</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -7928,7 +7929,7 @@
         <v>14</v>
       </c>
       <c r="B70" s="1">
-        <v>112.605983999999</v>
+        <v>147.394476</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>3</v>
@@ -7942,15 +7943,15 @@
         <v>14</v>
       </c>
       <c r="B71" s="1">
-        <v>114.83265599999901</v>
+        <v>144.26175599999999</v>
       </c>
       <c r="D71" s="1">
         <f>MIN(B66:B95)</f>
-        <v>112.605983999999</v>
+        <v>142.69539599999999</v>
       </c>
       <c r="E71" s="1">
         <f>MAX(B66:B95)</f>
-        <v>118.967904</v>
+        <v>150.213923999999</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -7958,7 +7959,7 @@
         <v>14</v>
       </c>
       <c r="B72" s="1">
-        <v>113.87836799999999</v>
+        <v>144.105119999999</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -7966,7 +7967,7 @@
         <v>14</v>
       </c>
       <c r="B73" s="1">
-        <v>113.87836799999999</v>
+        <v>144.26175599999999</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>5</v>
@@ -7980,15 +7981,15 @@
         <v>14</v>
       </c>
       <c r="B74" s="1">
-        <v>114.03741599999999</v>
+        <v>143.635212</v>
       </c>
       <c r="D74">
         <f>QUARTILE(B66:B95, 1)</f>
-        <v>113.71932</v>
+        <v>144.14427899999924</v>
       </c>
       <c r="E74">
         <f>QUARTILE(B66:B95, 2)</f>
-        <v>114.03741599999999</v>
+        <v>144.49671000000001</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -7996,7 +7997,7 @@
         <v>14</v>
       </c>
       <c r="B75" s="1">
-        <v>113.24217599999901</v>
+        <v>146.92456799999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -8004,7 +8005,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="1">
-        <v>114.991704</v>
+        <v>145.67148</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -8018,15 +8019,15 @@
         <v>14</v>
       </c>
       <c r="B77" s="1">
-        <v>114.51456</v>
+        <v>142.69539599999999</v>
       </c>
       <c r="D77">
         <f>QUARTILE(B66:B95, 3)</f>
-        <v>114.79289399999901</v>
+        <v>145.31904900000001</v>
       </c>
       <c r="E77">
         <f xml:space="preserve"> D77 - D74</f>
-        <v>1.073573999999013</v>
+        <v>1.1747700000007626</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -8034,7 +8035,7 @@
         <v>14</v>
       </c>
       <c r="B78" s="1">
-        <v>114.83265599999901</v>
+        <v>145.201572</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -8042,7 +8043,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="1">
-        <v>114.03741599999999</v>
+        <v>144.575028</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>16</v>
@@ -8056,15 +8057,15 @@
         <v>14</v>
       </c>
       <c r="B80" s="1">
-        <v>114.51456</v>
+        <v>145.35820799999999</v>
       </c>
       <c r="D80">
         <f>STDEV(B66:B95)</f>
-        <v>1.2030963084673518</v>
+        <v>1.428503263346357</v>
       </c>
       <c r="E80">
         <f xml:space="preserve"> (D80 / E68) * 100</f>
-        <v>1.0524082737757776</v>
+        <v>0.98593417366782432</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -8072,7 +8073,7 @@
         <v>14</v>
       </c>
       <c r="B81" s="1">
-        <v>114.03741599999999</v>
+        <v>144.73166399999999</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -8080,7 +8081,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="1">
-        <v>113.401224</v>
+        <v>146.14138800000001</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -8088,7 +8089,7 @@
         <v>14</v>
       </c>
       <c r="B83" s="1">
-        <v>113.71932</v>
+        <v>150.213923999999</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -8096,7 +8097,7 @@
         <v>14</v>
       </c>
       <c r="B84" s="1">
-        <v>113.87836799999999</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -8104,7 +8105,7 @@
         <v>14</v>
       </c>
       <c r="B85" s="1">
-        <v>113.71932</v>
+        <v>143.635212</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -8112,7 +8113,7 @@
         <v>14</v>
       </c>
       <c r="B86" s="1">
-        <v>114.03741599999999</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -8120,7 +8121,7 @@
         <v>14</v>
       </c>
       <c r="B87" s="1">
-        <v>114.196463999999</v>
+        <v>143.79184799999999</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -8128,7 +8129,7 @@
         <v>14</v>
       </c>
       <c r="B88" s="1">
-        <v>114.67360799999901</v>
+        <v>143.635212</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -8136,7 +8137,7 @@
         <v>14</v>
       </c>
       <c r="B89" s="1">
-        <v>115.150752</v>
+        <v>145.201572</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -8144,7 +8145,7 @@
         <v>14</v>
       </c>
       <c r="B90" s="1">
-        <v>113.71932</v>
+        <v>145.04493600000001</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -8152,7 +8153,7 @@
         <v>14</v>
       </c>
       <c r="B91" s="1">
-        <v>113.87836799999999</v>
+        <v>145.04493600000001</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -8160,7 +8161,7 @@
         <v>14</v>
       </c>
       <c r="B92" s="1">
-        <v>116.90028</v>
+        <v>144.105119999999</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -8168,7 +8169,7 @@
         <v>14</v>
       </c>
       <c r="B93" s="1">
-        <v>112.605983999999</v>
+        <v>143.478576</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -8176,7 +8177,7 @@
         <v>14</v>
       </c>
       <c r="B94" s="1">
-        <v>114.51456</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -8184,7 +8185,7 @@
         <v>14</v>
       </c>
       <c r="B95" s="1">
-        <v>113.71932</v>
+        <v>144.41839200000001</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -8200,7 +8201,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="1">
-        <v>108.467891999999</v>
+        <v>122.01944399999999</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -8208,7 +8209,7 @@
         <v>10</v>
       </c>
       <c r="B99" s="1">
-        <v>104.53219199999999</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -8216,7 +8217,7 @@
         <v>10</v>
       </c>
       <c r="B100" s="1">
-        <v>102.800484</v>
+        <v>123.585804</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -8224,7 +8225,7 @@
         <v>10</v>
       </c>
       <c r="B101" s="1">
-        <v>102.95791199999999</v>
+        <v>124.838892</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -8232,7 +8233,7 @@
         <v>10</v>
       </c>
       <c r="B102" s="1">
-        <v>102.95791199999999</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -8240,7 +8241,7 @@
         <v>10</v>
       </c>
       <c r="B103" s="1">
-        <v>101.226204</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -8248,7 +8249,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="1">
-        <v>102.48562800000001</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -8256,7 +8257,7 @@
         <v>10</v>
       </c>
       <c r="B105" s="1">
-        <v>101.698488</v>
+        <v>123.115895999999</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -8264,7 +8265,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="1">
-        <v>101.54106</v>
+        <v>124.21234800000001</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -8272,7 +8273,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="1">
-        <v>101.85591599999999</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -8280,7 +8281,7 @@
         <v>10</v>
       </c>
       <c r="B108" s="1">
-        <v>101.85591599999999</v>
+        <v>122.95926</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -8288,7 +8289,7 @@
         <v>10</v>
       </c>
       <c r="B109" s="1">
-        <v>102.170772</v>
+        <v>119.82653999999999</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -8296,7 +8297,7 @@
         <v>10</v>
       </c>
       <c r="B110" s="1">
-        <v>101.54106</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -8304,7 +8305,7 @@
         <v>10</v>
       </c>
       <c r="B111" s="1">
-        <v>101.54106</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -8312,7 +8313,7 @@
         <v>10</v>
       </c>
       <c r="B112" s="1">
-        <v>101.698488</v>
+        <v>124.682256</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -8320,7 +8321,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="1">
-        <v>116.969004</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -8328,7 +8329,7 @@
         <v>10</v>
       </c>
       <c r="B114" s="1">
-        <v>102.95791199999999</v>
+        <v>123.115895999999</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -8336,7 +8337,7 @@
         <v>10</v>
       </c>
       <c r="B115" s="1">
-        <v>101.85591599999999</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -8344,7 +8345,7 @@
         <v>10</v>
       </c>
       <c r="B116" s="1">
-        <v>101.54106</v>
+        <v>124.368984</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -8352,7 +8353,7 @@
         <v>10</v>
       </c>
       <c r="B117" s="1">
-        <v>102.3282</v>
+        <v>124.52562</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -8360,7 +8361,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="1">
-        <v>102.170772</v>
+        <v>123.115895999999</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -8368,7 +8369,7 @@
         <v>10</v>
       </c>
       <c r="B119" s="1">
-        <v>102.48562800000001</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -8376,7 +8377,7 @@
         <v>10</v>
       </c>
       <c r="B120" s="1">
-        <v>102.643056</v>
+        <v>124.055712</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -8384,7 +8385,7 @@
         <v>10</v>
       </c>
       <c r="B121" s="1">
-        <v>103.587623999999</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -8392,7 +8393,7 @@
         <v>10</v>
       </c>
       <c r="B122" s="1">
-        <v>101.85591599999999</v>
+        <v>122.489352</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -8400,7 +8401,7 @@
         <v>10</v>
       </c>
       <c r="B123" s="1">
-        <v>101.54106</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -8408,7 +8409,7 @@
         <v>10</v>
       </c>
       <c r="B124" s="1">
-        <v>101.698488</v>
+        <v>122.489352</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -8416,7 +8417,7 @@
         <v>10</v>
       </c>
       <c r="B125" s="1">
-        <v>102.013344</v>
+        <v>123.585804</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -8424,7 +8425,7 @@
         <v>10</v>
       </c>
       <c r="B126" s="1">
-        <v>101.38363200000001</v>
+        <v>119.043359999999</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -8432,7 +8433,7 @@
         <v>10</v>
       </c>
       <c r="B127" s="1">
-        <v>102.3282</v>
+        <v>123.429167999999</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -8440,7 +8441,7 @@
         <v>12</v>
       </c>
       <c r="B128" s="1">
-        <v>105.584256</v>
+        <v>127.814976</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -8448,7 +8449,7 @@
         <v>12</v>
       </c>
       <c r="B129" s="1">
-        <v>105.74208</v>
+        <v>134.70695999999899</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -8456,7 +8457,7 @@
         <v>12</v>
       </c>
       <c r="B130" s="1">
-        <v>105.74208</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -8464,7 +8465,7 @@
         <v>12</v>
       </c>
       <c r="B131" s="1">
-        <v>105.110784</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -8472,7 +8473,7 @@
         <v>12</v>
       </c>
       <c r="B132" s="1">
-        <v>105.26860799999901</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -8480,7 +8481,7 @@
         <v>12</v>
       </c>
       <c r="B133" s="1">
-        <v>105.110784</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -8488,7 +8489,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="1">
-        <v>105.584256</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -8496,7 +8497,7 @@
         <v>12</v>
       </c>
       <c r="B135" s="1">
-        <v>104.795136</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -8504,7 +8505,7 @@
         <v>12</v>
       </c>
       <c r="B136" s="1">
-        <v>104.795136</v>
+        <v>128.44152</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -8512,7 +8513,7 @@
         <v>12</v>
       </c>
       <c r="B137" s="1">
-        <v>104.479488</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -8520,7 +8521,7 @@
         <v>12</v>
       </c>
       <c r="B138" s="1">
-        <v>105.26860799999901</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -8528,7 +8529,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="1">
-        <v>106.84684799999999</v>
+        <v>124.838892</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -8536,7 +8537,7 @@
         <v>12</v>
       </c>
       <c r="B140" s="1">
-        <v>105.74208</v>
+        <v>136.89986399999901</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -8544,7 +8545,7 @@
         <v>12</v>
       </c>
       <c r="B141" s="1">
-        <v>106.057728</v>
+        <v>128.59815599999999</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -8552,7 +8553,7 @@
         <v>12</v>
       </c>
       <c r="B142" s="1">
-        <v>105.110784</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -8560,7 +8561,7 @@
         <v>12</v>
       </c>
       <c r="B143" s="1">
-        <v>105.426431999999</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -8568,7 +8569,7 @@
         <v>12</v>
       </c>
       <c r="B144" s="1">
-        <v>104.95296</v>
+        <v>128.28488399999901</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -8576,7 +8577,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="1">
-        <v>105.426431999999</v>
+        <v>127.814976</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -8584,7 +8585,7 @@
         <v>12</v>
       </c>
       <c r="B146" s="1">
-        <v>104.795136</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -8592,7 +8593,7 @@
         <v>12</v>
       </c>
       <c r="B147" s="1">
-        <v>104.95296</v>
+        <v>128.75479200000001</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -8600,7 +8601,7 @@
         <v>12</v>
       </c>
       <c r="B148" s="1">
-        <v>104.95296</v>
+        <v>132.98396399999999</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -8608,7 +8609,7 @@
         <v>12</v>
       </c>
       <c r="B149" s="1">
-        <v>105.584256</v>
+        <v>128.44152</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -8616,7 +8617,7 @@
         <v>12</v>
       </c>
       <c r="B150" s="1">
-        <v>104.95296</v>
+        <v>129.537972</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -8624,7 +8625,7 @@
         <v>12</v>
       </c>
       <c r="B151" s="1">
-        <v>105.426431999999</v>
+        <v>131.104332</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -8632,7 +8633,7 @@
         <v>12</v>
       </c>
       <c r="B152" s="1">
-        <v>104.795136</v>
+        <v>130.32115200000001</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -8640,7 +8641,7 @@
         <v>12</v>
       </c>
       <c r="B153" s="1">
-        <v>105.110784</v>
+        <v>134.23705200000001</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -8648,7 +8649,7 @@
         <v>12</v>
       </c>
       <c r="B154" s="1">
-        <v>105.110784</v>
+        <v>129.06806399999999</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -8656,7 +8657,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="1">
-        <v>105.110784</v>
+        <v>133.297236</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -8664,7 +8665,7 @@
         <v>12</v>
       </c>
       <c r="B156" s="1">
-        <v>104.16383999999999</v>
+        <v>124.52562</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -8672,7 +8673,7 @@
         <v>12</v>
       </c>
       <c r="B157" s="1">
-        <v>105.89990400000001</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -8680,7 +8681,7 @@
         <v>14</v>
       </c>
       <c r="B158" s="1">
-        <v>113.401224</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -8688,7 +8689,7 @@
         <v>14</v>
       </c>
       <c r="B159" s="1">
-        <v>114.83265599999901</v>
+        <v>145.82811599999999</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -8696,7 +8697,7 @@
         <v>14</v>
       </c>
       <c r="B160" s="1">
-        <v>114.83265599999901</v>
+        <v>144.88829999999999</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -8704,7 +8705,7 @@
         <v>14</v>
       </c>
       <c r="B161" s="1">
-        <v>118.967904</v>
+        <v>145.35820799999999</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -8712,7 +8713,7 @@
         <v>14</v>
       </c>
       <c r="B162" s="1">
-        <v>112.605983999999</v>
+        <v>147.394476</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -8720,7 +8721,7 @@
         <v>14</v>
       </c>
       <c r="B163" s="1">
-        <v>114.83265599999901</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -8728,7 +8729,7 @@
         <v>14</v>
       </c>
       <c r="B164" s="1">
-        <v>113.87836799999999</v>
+        <v>144.105119999999</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -8736,7 +8737,7 @@
         <v>14</v>
       </c>
       <c r="B165" s="1">
-        <v>113.87836799999999</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -8744,7 +8745,7 @@
         <v>14</v>
       </c>
       <c r="B166" s="1">
-        <v>114.03741599999999</v>
+        <v>143.635212</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -8752,7 +8753,7 @@
         <v>14</v>
       </c>
       <c r="B167" s="1">
-        <v>113.24217599999901</v>
+        <v>146.92456799999999</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -8760,7 +8761,7 @@
         <v>14</v>
       </c>
       <c r="B168" s="1">
-        <v>114.991704</v>
+        <v>145.67148</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -8768,7 +8769,7 @@
         <v>14</v>
       </c>
       <c r="B169" s="1">
-        <v>114.51456</v>
+        <v>142.69539599999999</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -8776,7 +8777,7 @@
         <v>14</v>
       </c>
       <c r="B170" s="1">
-        <v>114.83265599999901</v>
+        <v>145.201572</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -8784,7 +8785,7 @@
         <v>14</v>
       </c>
       <c r="B171" s="1">
-        <v>114.03741599999999</v>
+        <v>144.575028</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -8792,7 +8793,7 @@
         <v>14</v>
       </c>
       <c r="B172" s="1">
-        <v>114.51456</v>
+        <v>145.35820799999999</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -8800,7 +8801,7 @@
         <v>14</v>
       </c>
       <c r="B173" s="1">
-        <v>114.03741599999999</v>
+        <v>144.73166399999999</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -8808,7 +8809,7 @@
         <v>14</v>
       </c>
       <c r="B174" s="1">
-        <v>113.401224</v>
+        <v>146.14138800000001</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -8816,7 +8817,7 @@
         <v>14</v>
       </c>
       <c r="B175" s="1">
-        <v>113.71932</v>
+        <v>150.213923999999</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -8824,7 +8825,7 @@
         <v>14</v>
       </c>
       <c r="B176" s="1">
-        <v>113.87836799999999</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -8832,7 +8833,7 @@
         <v>14</v>
       </c>
       <c r="B177" s="1">
-        <v>113.71932</v>
+        <v>143.635212</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -8840,7 +8841,7 @@
         <v>14</v>
       </c>
       <c r="B178" s="1">
-        <v>114.03741599999999</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -8848,7 +8849,7 @@
         <v>14</v>
       </c>
       <c r="B179" s="1">
-        <v>114.196463999999</v>
+        <v>143.79184799999999</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
@@ -8856,7 +8857,7 @@
         <v>14</v>
       </c>
       <c r="B180" s="1">
-        <v>114.67360799999901</v>
+        <v>143.635212</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -8864,7 +8865,7 @@
         <v>14</v>
       </c>
       <c r="B181" s="1">
-        <v>115.150752</v>
+        <v>145.201572</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -8872,7 +8873,7 @@
         <v>14</v>
       </c>
       <c r="B182" s="1">
-        <v>113.71932</v>
+        <v>145.04493600000001</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -8880,7 +8881,7 @@
         <v>14</v>
       </c>
       <c r="B183" s="1">
-        <v>113.87836799999999</v>
+        <v>145.04493600000001</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -8888,7 +8889,7 @@
         <v>14</v>
       </c>
       <c r="B184" s="1">
-        <v>116.90028</v>
+        <v>144.105119999999</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -8896,7 +8897,7 @@
         <v>14</v>
       </c>
       <c r="B185" s="1">
-        <v>112.605983999999</v>
+        <v>143.478576</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -8904,7 +8905,7 @@
         <v>14</v>
       </c>
       <c r="B186" s="1">
-        <v>114.51456</v>
+        <v>144.26175599999999</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -8912,7 +8913,7 @@
         <v>14</v>
       </c>
       <c r="B187" s="1">
-        <v>113.71932</v>
+        <v>144.41839200000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>